<commit_message>
Add STATIC_ROOT for deployment
</commit_message>
<xml_diff>
--- a/FinTrak_Report.xlsx
+++ b/FinTrak_Report.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,34 +476,227 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>bakary</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>500.00</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>45962</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>for morning tea</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>sugar</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>200.00</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>45963</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>gfhg</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>54353.00</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>45967</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>16</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>play</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>45962</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>glay</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1230.00</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>45989</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>200.00</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>45988</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>it was nessesary to buy</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>12000.00</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>38936</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>34</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>123000.00</t>
         </is>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>45975</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Add kr Bhai</t>
-        </is>
-      </c>
+      <c r="F9" s="2" t="n">
+        <v>45988</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>